<commit_message>
Update Fujiya Instruments OSB, OFB v1.3
</commit_message>
<xml_diff>
--- a/Fujiya Instruments/Organic Fingered Bass/xlsx/OFB.xlsx
+++ b/Fujiya Instruments/Organic Fingered Bass/xlsx/OFB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6645" windowWidth="28830" windowHeight="6705" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="6645" windowWidth="28830" windowHeight="6705" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Organic Fingered Bass (Main)" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="165">
   <si>
     <t>Name</t>
   </si>
@@ -575,12 +575,6 @@
     <t>Gliss Down</t>
   </si>
   <si>
-    <t>Stop Noise 1</t>
-  </si>
-  <si>
-    <t>Stop Noise 2</t>
-  </si>
-  <si>
     <t>Slide Down</t>
   </si>
   <si>
@@ -606,6 +600,32 @@
   </si>
   <si>
     <t>String - 1st</t>
+  </si>
+  <si>
+    <t>Hand Stop Noise</t>
+  </si>
+  <si>
+    <t>Hand Stop Noise</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Noiseless Stop</t>
+  </si>
+  <si>
+    <t>Noiseless Stop</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Slide Down</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Mute Stop</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Mute Stop</t>
+    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
@@ -1238,7 +1258,7 @@
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:G8"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75"/>
@@ -3112,12 +3132,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K129"/>
+  <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75"/>
@@ -3192,7 +3212,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
@@ -3207,7 +3227,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G3" s="12">
         <v>120</v>
@@ -3219,13 +3239,13 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>12</v>
@@ -3234,7 +3254,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G4" s="12">
         <v>120</v>
@@ -3246,13 +3266,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>12</v>
@@ -3261,7 +3281,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G5" s="12">
         <v>120</v>
@@ -3272,13 +3292,27 @@
       <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="1"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+      <c r="A6" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="12">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="12">
+        <v>120</v>
+      </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -4883,26 +4917,39 @@
       <c r="J129" s="12"/>
       <c r="K129" s="12"/>
     </row>
+    <row r="130" spans="1:11">
+      <c r="A130" s="1"/>
+      <c r="B130" s="12"/>
+      <c r="C130" s="2"/>
+      <c r="D130" s="13"/>
+      <c r="E130" s="12"/>
+      <c r="F130" s="12"/>
+      <c r="G130" s="12"/>
+      <c r="H130" s="12"/>
+      <c r="I130" s="12"/>
+      <c r="J130" s="12"/>
+      <c r="K130" s="12"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="6"/>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K2:K129">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K2:K130">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J2:J129">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J2:J130">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G2:G129">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G2:G130">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H2:I129">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H2:I130">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B129">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B130">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4920,7 +4967,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>F2:F129</xm:sqref>
+          <xm:sqref>F2:F130</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -4929,7 +4976,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>E2:E129</xm:sqref>
+          <xm:sqref>E2:E130</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -4938,7 +4985,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D2:D129</xm:sqref>
+          <xm:sqref>D2:D130</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4953,7 +5000,7 @@
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75"/>
@@ -5028,13 +5075,13 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>12</v>
@@ -5055,13 +5102,13 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>12</v>
@@ -5082,13 +5129,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>12</v>
@@ -6786,10 +6833,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75"/>
@@ -6864,13 +6911,13 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>12</v>
@@ -6891,13 +6938,13 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>12</v>
@@ -6918,13 +6965,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>12</v>
@@ -6945,13 +6992,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B6" s="12">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>12</v>
@@ -6972,13 +7019,13 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B7" s="12">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Added: Fujiya Instruments OPB Updated: OFB, OSB (Stop Noise)
</commit_message>
<xml_diff>
--- a/Fujiya Instruments/Organic Fingered Bass/xlsx/OFB.xlsx
+++ b/Fujiya Instruments/Organic Fingered Bass/xlsx/OFB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6645" windowWidth="28830" windowHeight="6705" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="28830" windowHeight="6660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Organic Fingered Bass (Main)" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="174">
   <si>
     <t>Name</t>
   </si>
@@ -575,9 +575,6 @@
     <t>Gliss Down</t>
   </si>
   <si>
-    <t>Slide Down</t>
-  </si>
-  <si>
     <t>Finger - Auto</t>
   </si>
   <si>
@@ -602,30 +599,55 @@
     <t>String - 1st</t>
   </si>
   <si>
-    <t>Hand Stop Noise</t>
-  </si>
-  <si>
-    <t>Hand Stop Noise</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Noiseless Stop</t>
-  </si>
-  <si>
-    <t>Noiseless Stop</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Slide Down</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Mute Stop</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Mute Stop</t>
-    <phoneticPr fontId="6"/>
+    <t>Slide Down (vel 32)</t>
+  </si>
+  <si>
+    <t>Slide Down (vel 64)</t>
+  </si>
+  <si>
+    <t>Slide Down (vel 96)</t>
+  </si>
+  <si>
+    <t>Slide Down (vel 127)</t>
+  </si>
+  <si>
+    <t>Noiseless Stop (vel 31)</t>
+  </si>
+  <si>
+    <t>Noiseless Stop (vel 64)</t>
+  </si>
+  <si>
+    <t>Noiseless Stop (vel 96)</t>
+  </si>
+  <si>
+    <t>Noiseless Stop (vel 127)</t>
+  </si>
+  <si>
+    <t>Hand Stop Noise (vel 31)</t>
+  </si>
+  <si>
+    <t>Hand Stop Noise (vel 64)</t>
+  </si>
+  <si>
+    <t>Hand Stop Noise (vel 96)</t>
+  </si>
+  <si>
+    <t>Hand Stop Noise (vel 127)</t>
+  </si>
+  <si>
+    <t>Mute Stop (vel 31)</t>
+  </si>
+  <si>
+    <t>Mute Stop (vel 64)</t>
+  </si>
+  <si>
+    <t>Mute Stop (vel 96)</t>
+  </si>
+  <si>
+    <t>Mute Stop (vel 127)</t>
+  </si>
+  <si>
+    <t>Slide Down (vel 31)</t>
   </si>
 </sst>
 </file>
@@ -3132,12 +3154,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K130"/>
+  <dimension ref="A1:K139"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75"/>
@@ -3212,13 +3234,13 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>12</v>
@@ -3230,7 +3252,7 @@
         <v>45</v>
       </c>
       <c r="G3" s="12">
-        <v>120</v>
+        <v>31</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -3239,13 +3261,13 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>12</v>
@@ -3254,10 +3276,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G4" s="12">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -3272,7 +3294,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>12</v>
@@ -3281,10 +3303,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G5" s="12">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -3293,13 +3315,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B6" s="12">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>12</v>
@@ -3308,10 +3330,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G6" s="12">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -3319,156 +3341,324 @@
       <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="1"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
+      <c r="A7" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="12">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="12">
+        <v>1</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="12">
+        <v>31</v>
+      </c>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="1"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="A8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="12">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="12">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="12">
+        <v>64</v>
+      </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="1"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
+      <c r="A9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" s="12">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="12">
+        <v>1</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="12">
+        <v>96</v>
+      </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="1"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+      <c r="A10" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="12">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="12">
+        <v>127</v>
+      </c>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="1"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
+      <c r="A11" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="12">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="12">
+        <v>1</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="12">
+        <v>31</v>
+      </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="1"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+      <c r="A12" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12" s="12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="12">
+        <v>64</v>
+      </c>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="1"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
+      <c r="A13" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="12">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="12">
+        <v>1</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="12">
+        <v>96</v>
+      </c>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="1"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="A14" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14" s="12">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="12">
+        <v>1</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="12">
+        <v>127</v>
+      </c>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="1"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="A15" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B15" s="12">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="12">
+        <v>1</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="12">
+        <v>31</v>
+      </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="1"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="A16" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="12">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="12">
+        <v>1</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="12">
+        <v>64</v>
+      </c>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="1"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
+      <c r="A17" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" s="12">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="12">
+        <v>1</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="12">
+        <v>96</v>
+      </c>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="1"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
+      <c r="A18" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" s="12">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="12">
+        <v>1</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="12">
+        <v>127</v>
+      </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
@@ -4930,26 +5120,143 @@
       <c r="J130" s="12"/>
       <c r="K130" s="12"/>
     </row>
+    <row r="131" spans="1:11">
+      <c r="A131" s="1"/>
+      <c r="B131" s="12"/>
+      <c r="C131" s="2"/>
+      <c r="D131" s="13"/>
+      <c r="E131" s="12"/>
+      <c r="F131" s="12"/>
+      <c r="G131" s="12"/>
+      <c r="H131" s="12"/>
+      <c r="I131" s="12"/>
+      <c r="J131" s="12"/>
+      <c r="K131" s="12"/>
+    </row>
+    <row r="132" spans="1:11">
+      <c r="A132" s="1"/>
+      <c r="B132" s="12"/>
+      <c r="C132" s="2"/>
+      <c r="D132" s="13"/>
+      <c r="E132" s="12"/>
+      <c r="F132" s="12"/>
+      <c r="G132" s="12"/>
+      <c r="H132" s="12"/>
+      <c r="I132" s="12"/>
+      <c r="J132" s="12"/>
+      <c r="K132" s="12"/>
+    </row>
+    <row r="133" spans="1:11">
+      <c r="A133" s="1"/>
+      <c r="B133" s="12"/>
+      <c r="C133" s="2"/>
+      <c r="D133" s="13"/>
+      <c r="E133" s="12"/>
+      <c r="F133" s="12"/>
+      <c r="G133" s="12"/>
+      <c r="H133" s="12"/>
+      <c r="I133" s="12"/>
+      <c r="J133" s="12"/>
+      <c r="K133" s="12"/>
+    </row>
+    <row r="134" spans="1:11">
+      <c r="A134" s="1"/>
+      <c r="B134" s="12"/>
+      <c r="C134" s="2"/>
+      <c r="D134" s="13"/>
+      <c r="E134" s="12"/>
+      <c r="F134" s="12"/>
+      <c r="G134" s="12"/>
+      <c r="H134" s="12"/>
+      <c r="I134" s="12"/>
+      <c r="J134" s="12"/>
+      <c r="K134" s="12"/>
+    </row>
+    <row r="135" spans="1:11">
+      <c r="A135" s="1"/>
+      <c r="B135" s="12"/>
+      <c r="C135" s="2"/>
+      <c r="D135" s="13"/>
+      <c r="E135" s="12"/>
+      <c r="F135" s="12"/>
+      <c r="G135" s="12"/>
+      <c r="H135" s="12"/>
+      <c r="I135" s="12"/>
+      <c r="J135" s="12"/>
+      <c r="K135" s="12"/>
+    </row>
+    <row r="136" spans="1:11">
+      <c r="A136" s="1"/>
+      <c r="B136" s="12"/>
+      <c r="C136" s="2"/>
+      <c r="D136" s="13"/>
+      <c r="E136" s="12"/>
+      <c r="F136" s="12"/>
+      <c r="G136" s="12"/>
+      <c r="H136" s="12"/>
+      <c r="I136" s="12"/>
+      <c r="J136" s="12"/>
+      <c r="K136" s="12"/>
+    </row>
+    <row r="137" spans="1:11">
+      <c r="A137" s="1"/>
+      <c r="B137" s="12"/>
+      <c r="C137" s="2"/>
+      <c r="D137" s="13"/>
+      <c r="E137" s="12"/>
+      <c r="F137" s="12"/>
+      <c r="G137" s="12"/>
+      <c r="H137" s="12"/>
+      <c r="I137" s="12"/>
+      <c r="J137" s="12"/>
+      <c r="K137" s="12"/>
+    </row>
+    <row r="138" spans="1:11">
+      <c r="A138" s="1"/>
+      <c r="B138" s="12"/>
+      <c r="C138" s="2"/>
+      <c r="D138" s="13"/>
+      <c r="E138" s="12"/>
+      <c r="F138" s="12"/>
+      <c r="G138" s="12"/>
+      <c r="H138" s="12"/>
+      <c r="I138" s="12"/>
+      <c r="J138" s="12"/>
+      <c r="K138" s="12"/>
+    </row>
+    <row r="139" spans="1:11">
+      <c r="A139" s="1"/>
+      <c r="B139" s="12"/>
+      <c r="C139" s="2"/>
+      <c r="D139" s="13"/>
+      <c r="E139" s="12"/>
+      <c r="F139" s="12"/>
+      <c r="G139" s="12"/>
+      <c r="H139" s="12"/>
+      <c r="I139" s="12"/>
+      <c r="J139" s="12"/>
+      <c r="K139" s="12"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="6"/>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K2:K130">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K2:K139">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J2:J130">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J2:J139">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G2:G130">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G2:G139">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H2:I130">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H2:I139">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B130">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B139">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4967,7 +5274,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>F2:F130</xm:sqref>
+          <xm:sqref>F2:F139</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -4976,7 +5283,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>E2:E130</xm:sqref>
+          <xm:sqref>E2:E139</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -4985,7 +5292,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D2:D130</xm:sqref>
+          <xm:sqref>D2:D139</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5075,13 +5382,13 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>12</v>
@@ -5102,13 +5409,13 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>12</v>
@@ -5129,13 +5436,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>12</v>
@@ -6911,13 +7218,13 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>12</v>
@@ -6938,13 +7245,13 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>12</v>
@@ -6965,13 +7272,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>12</v>
@@ -6992,13 +7299,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B6" s="12">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>12</v>
@@ -7019,13 +7326,13 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" s="12">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>12</v>

</xml_diff>